<commit_message>
SOH curve vs Ah implemented for NMC
</commit_message>
<xml_diff>
--- a/src/pymgrid/modules/battery/transition_models/data/NMC-SOHAh.xlsx
+++ b/src/pymgrid/modules/battery/transition_models/data/NMC-SOHAh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive - University of Pisa\Documenti\GitHub\microgrid-simulator\src\pymgrid\modules\battery\transition_models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E3F7DF-310B-4F06-8057-2C2F9A7FBA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D3F81C-DEBC-4C11-BC1F-18AAE64B4697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:X75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,6 +502,478 @@
         <v>81.8</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1842</v>
+      </c>
+      <c r="B17">
+        <v>81.599999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2097.1999999999998</v>
+      </c>
+      <c r="B18">
+        <v>81.400000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2352.4</v>
+      </c>
+      <c r="B19">
+        <v>81.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2607.6</v>
+      </c>
+      <c r="B20">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2862.8</v>
+      </c>
+      <c r="B21">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3118</v>
+      </c>
+      <c r="B22">
+        <v>80.599999999999994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>3373.2</v>
+      </c>
+      <c r="B23">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>3628.4</v>
+      </c>
+      <c r="B24">
+        <v>80.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3883.6</v>
+      </c>
+      <c r="B25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>4138.8</v>
+      </c>
+      <c r="B26">
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>4394</v>
+      </c>
+      <c r="B27">
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>4649.2</v>
+      </c>
+      <c r="B28">
+        <v>79.400000000000006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>4904.3999999999996</v>
+      </c>
+      <c r="B29">
+        <v>79.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>5159.6000000000004</v>
+      </c>
+      <c r="B30">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>5414.8</v>
+      </c>
+      <c r="B31">
+        <v>78.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>5670</v>
+      </c>
+      <c r="B32">
+        <v>78.599999999999994</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>5925.2</v>
+      </c>
+      <c r="B33">
+        <v>78.399999999999906</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>6180.4</v>
+      </c>
+      <c r="B34">
+        <v>78.199999999999903</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>6435.6</v>
+      </c>
+      <c r="B35">
+        <v>77.999999999999901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>6690.8</v>
+      </c>
+      <c r="B36">
+        <v>77.799999999999898</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>6946</v>
+      </c>
+      <c r="B37">
+        <v>77.599999999999895</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>7201.2</v>
+      </c>
+      <c r="B38">
+        <v>77.399999999999906</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>7456.4</v>
+      </c>
+      <c r="B39">
+        <v>77.199999999999903</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>7711.6</v>
+      </c>
+      <c r="B40">
+        <v>76.999999999999901</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>7966.8</v>
+      </c>
+      <c r="B41">
+        <v>76.799999999999898</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>8222</v>
+      </c>
+      <c r="B42">
+        <v>76.599999999999895</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>8477.2000000000007</v>
+      </c>
+      <c r="B43">
+        <v>76.399999999999906</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>8732.4</v>
+      </c>
+      <c r="B44">
+        <v>76.199999999999903</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>8987.6</v>
+      </c>
+      <c r="B45">
+        <v>75.999999999999901</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>9242.7999999999993</v>
+      </c>
+      <c r="B46">
+        <v>75.799999999999898</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>9498</v>
+      </c>
+      <c r="B47">
+        <v>75.599999999999895</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>9753.2000000000007</v>
+      </c>
+      <c r="B48">
+        <v>75.399999999999906</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>10008.4</v>
+      </c>
+      <c r="B49">
+        <v>75.199999999999903</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>10263.6</v>
+      </c>
+      <c r="B50">
+        <v>74.999999999999901</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>10518.8</v>
+      </c>
+      <c r="B51">
+        <v>74.799999999999898</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>10774</v>
+      </c>
+      <c r="B52">
+        <v>74.599999999999895</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>11029.2</v>
+      </c>
+      <c r="B53">
+        <v>74.399999999999906</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>11284.4</v>
+      </c>
+      <c r="B54">
+        <v>74.199999999999903</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>11539.6</v>
+      </c>
+      <c r="B55">
+        <v>73.999999999999901</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>11794.8</v>
+      </c>
+      <c r="B56">
+        <v>73.799999999999898</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>12050</v>
+      </c>
+      <c r="B57">
+        <v>73.599999999999895</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>12305.2</v>
+      </c>
+      <c r="B58">
+        <v>73.399999999999906</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>12560.4</v>
+      </c>
+      <c r="B59">
+        <v>73.199999999999903</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>12815.6</v>
+      </c>
+      <c r="B60">
+        <v>72.999999999999901</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>13070.8</v>
+      </c>
+      <c r="B61">
+        <v>72.799999999999898</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>13326</v>
+      </c>
+      <c r="B62">
+        <v>72.599999999999895</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>13581.2</v>
+      </c>
+      <c r="B63">
+        <v>72.399999999999906</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>13836.4</v>
+      </c>
+      <c r="B64">
+        <v>72.199999999999903</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>14091.6</v>
+      </c>
+      <c r="B65">
+        <v>71.999999999999901</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>14346.8</v>
+      </c>
+      <c r="B66">
+        <v>71.799999999999898</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>14602</v>
+      </c>
+      <c r="B67">
+        <v>71.599999999999895</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>14857.2</v>
+      </c>
+      <c r="B68">
+        <v>71.399999999999807</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>15112.4</v>
+      </c>
+      <c r="B69">
+        <v>71.199999999999804</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>15367.6</v>
+      </c>
+      <c r="B70">
+        <v>70.999999999999801</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>15622.8</v>
+      </c>
+      <c r="B71">
+        <v>70.799999999999798</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>15878</v>
+      </c>
+      <c r="B72">
+        <v>70.599999999999795</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>16133.2</v>
+      </c>
+      <c r="B73">
+        <v>70.399999999999807</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>16388.400000000001</v>
+      </c>
+      <c r="B74">
+        <v>70.199999999999804</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>16643.599999999999</v>
+      </c>
+      <c r="B75">
+        <v>69.999999999999801</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>